<commit_message>
This is my first commit
</commit_message>
<xml_diff>
--- a/testdata/ExcelWrite.xlsx
+++ b/testdata/ExcelWrite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="24">
   <si>
     <t>Niva Bupa (formerly known as Max Bupa)</t>
   </si>
@@ -417,24 +417,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
       <c r="C1" t="s" s="0">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">

</xml_diff>